<commit_message>
se termino el ejercicio para obtener la nota en uipath academy
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t xml:space="preserve">acme-test.uipath.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHA1URL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://codebeautify.org/sha1-hash-generator</t>
   </si>
   <si>
     <t xml:space="preserve">MaxRetryNumber</t>
@@ -259,8 +265,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,8 +286,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -304,100 +318,107 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="81.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="43.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="81.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="1" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1412,181 +1433,181 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="75.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="75.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="1" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>16</v>
+      <c r="C2" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>18</v>
+      <c r="C3" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="0" t="n">
+      <c r="A14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>41</v>
+      <c r="C14" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="0" t="n">
+      <c r="A15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>43</v>
+      <c r="C15" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="0" t="b">
+      <c r="A17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>45</v>
+      <c r="C17" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2584,50 +2605,50 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="0" width="65.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="60.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="4" style="1" width="65.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
+      <c r="C1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4"/>
+      <c r="A2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>